<commit_message>
ensayo ajuste camilo - oliver
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion02/EsqueletoGuion_CN_06_02_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion02/EsqueletoGuion_CN_06_02_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="11760" tabRatio="729"/>
+    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="11760" tabRatio="729" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="77">
   <si>
     <t>FICHA</t>
   </si>
@@ -248,6 +248,15 @@
   </si>
   <si>
     <t>Ciencias Naturales</t>
+  </si>
+  <si>
+    <t>1° ESO</t>
+  </si>
+  <si>
+    <t>Los seres vivos</t>
+  </si>
+  <si>
+    <t>CN_07_06</t>
   </si>
 </sst>
 </file>
@@ -1499,7 +1508,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1509,7 +1518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1582,8 +1591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1645,20 +1654,20 @@
       <c r="L2"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3">
-        <v>6</v>
+      <c r="A3" t="s">
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>69</v>
+      <c r="E3" t="s">
+        <v>76</v>
       </c>
       <c r="F3">
         <v>3</v>

</xml_diff>

<commit_message>
Ajustes Guion 02 grado 06 y guion 09 grado 09
Ajustes finales. Grado 06 Guion 02 y Grado 09 Guion 09. Solo falta
ajuste de correccion de estilo en manuscrito y recursos guion 09 grado
09
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion02/EsqueletoGuion_CN_06_02_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion02/EsqueletoGuion_CN_06_02_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="11760" tabRatio="729" activeTab="1"/>
+    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="11760" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725" iterateCount="2" iterateDelta="10"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="87">
   <si>
     <t>FICHA</t>
   </si>
@@ -112,9 +112,6 @@
     <t>Practica</t>
   </si>
   <si>
-    <t>¿Cuáles son las funciones vitales de una célula?</t>
-  </si>
-  <si>
     <t>Sí</t>
   </si>
   <si>
@@ -145,9 +142,6 @@
     <t>La estructura de la célula</t>
   </si>
   <si>
-    <t>Relaciona las diferentes partes de la célula con la definición correspondiente</t>
-  </si>
-  <si>
     <t>Tipos de células</t>
   </si>
   <si>
@@ -163,12 +157,6 @@
     <t>Célula procariota y eucariota</t>
   </si>
   <si>
-    <t>Células procariotas y eucariotas</t>
-  </si>
-  <si>
-    <t>La definición de célula</t>
-  </si>
-  <si>
     <t>Organismos unicelulares y pluricelulares</t>
   </si>
   <si>
@@ -178,18 +166,9 @@
     <t>Los órganos</t>
   </si>
   <si>
-    <t>Cuáles son los niveles de organización en los organismos</t>
-  </si>
-  <si>
     <t>La forma y el tamaño de las células</t>
   </si>
   <si>
-    <t>Reconoce diferentes tipos de célula</t>
-  </si>
-  <si>
-    <t>Los seres unicelulares y pluricelulares</t>
-  </si>
-  <si>
     <t>El microscopio</t>
   </si>
   <si>
@@ -214,15 +193,9 @@
     <t>Preparación de una muestra para el microscopio</t>
   </si>
   <si>
-    <t>Observación en el microscopio de células animales y vegetales</t>
-  </si>
-  <si>
     <t>Utilización del microscopio y la lupa binocular</t>
   </si>
   <si>
-    <t>Fin de unidad</t>
-  </si>
-  <si>
     <t>Mapa conceptual</t>
   </si>
   <si>
@@ -235,12 +208,6 @@
     <t>CN</t>
   </si>
   <si>
-    <t>CN_06_02</t>
-  </si>
-  <si>
-    <t>La célula es la unidad fundamental de vida. Los seres vivos están hechos de células. Adéntrate en este tema y descubre de qué está hecha la materia viva.</t>
-  </si>
-  <si>
     <t>CN_06_02_CO</t>
   </si>
   <si>
@@ -257,6 +224,69 @@
   </si>
   <si>
     <t>CN_07_06</t>
+  </si>
+  <si>
+    <t>¿Cuáles son las funciones vitales de la célula?</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>MN_3C_11</t>
+  </si>
+  <si>
+    <t>3° ESO</t>
+  </si>
+  <si>
+    <t>BG</t>
+  </si>
+  <si>
+    <t>El cuerpo humano</t>
+  </si>
+  <si>
+    <t>BG_09_01</t>
+  </si>
+  <si>
+    <t>Identifica las partes de las células y sus funciones</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La definición de célula</t>
+  </si>
+  <si>
+    <t>¿Cuáles son los niveles de organización de los organismos?</t>
+  </si>
+  <si>
+    <t>Reconoce diferentes tipos de células</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Los seres unicelulares y pluricelulares</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: El microscopio</t>
+  </si>
+  <si>
+    <t>Competencias: construcción de los distintos modelos celulares</t>
+  </si>
+  <si>
+    <t>Competencias: preparación de una muestra para el microscopio</t>
+  </si>
+  <si>
+    <t>Competencias: Preparación de una muestra para el microscopio</t>
+  </si>
+  <si>
+    <t>Competencias: diferenciación del tipo celular al microscopio</t>
+  </si>
+  <si>
+    <t>Diferenciación del tipo celular al microscopio</t>
+  </si>
+  <si>
+    <t>Competencias: utilización del microscopio y la lupa binocular</t>
+  </si>
+  <si>
+    <t>La célula es la unidad fundamental de vida. La materia que compone a los seres vivos necesita para su estructura y sus funciones a las células.</t>
+  </si>
+  <si>
+    <t>Fin de tema</t>
   </si>
 </sst>
 </file>
@@ -780,7 +810,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -826,7 +856,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1519,7 +1548,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1541,7 +1570,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1549,7 +1578,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1557,7 +1586,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1573,7 +1602,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1591,8 +1620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1632,16 +1661,16 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" t="s">
         <v>68</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1655,39 +1684,39 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="F3">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4">
-        <v>6</v>
+      <c r="A4" t="s">
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>72</v>
       </c>
       <c r="F4">
         <v>4</v>
@@ -1698,36 +1727,36 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" t="s">
         <v>68</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="F5">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6">
-        <v>6</v>
+      <c r="A6" t="s">
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>69</v>
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>65</v>
       </c>
       <c r="F6">
         <v>8</v>
@@ -1738,16 +1767,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" t="s">
         <v>68</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="F7">
         <v>9</v>
@@ -1758,16 +1787,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
         <v>68</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="F8">
         <v>10</v>
@@ -1778,16 +1807,16 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" t="s">
         <v>68</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="F9">
         <v>11</v>
@@ -1799,16 +1828,16 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" t="s">
         <v>68</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="F10">
         <v>12</v>
@@ -1820,16 +1849,16 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" t="s">
         <v>68</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="F11">
         <v>13</v>
@@ -1841,16 +1870,16 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" t="s">
         <v>68</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="F12">
         <v>14</v>
@@ -1862,16 +1891,16 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
         <v>68</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="F13">
         <v>15</v>
@@ -1882,16 +1911,16 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" t="s">
         <v>68</v>
-      </c>
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="F14">
         <v>16</v>
@@ -1902,16 +1931,16 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" t="s">
         <v>68</v>
-      </c>
-      <c r="C15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="F15">
         <v>17</v>
@@ -1922,16 +1951,16 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" t="s">
         <v>68</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="F16">
         <v>18</v>
@@ -1942,16 +1971,16 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" t="s">
         <v>68</v>
-      </c>
-      <c r="C17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="F17">
         <v>19</v>
@@ -1962,16 +1991,16 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" t="s">
         <v>68</v>
-      </c>
-      <c r="C18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="F18">
         <v>20</v>
@@ -1979,7 +2008,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2015,10 +2044,10 @@
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1">
       <c r="A2" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -2026,10 +2055,10 @@
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C3">
         <v>6</v>
@@ -2037,10 +2066,10 @@
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C4">
         <v>7</v>
@@ -2048,10 +2077,10 @@
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1">
       <c r="A5" s="19" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5">
         <v>21</v>
@@ -2059,10 +2088,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="19" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6">
         <v>22</v>
@@ -2090,7 +2119,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A21"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2116,21 +2145,21 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="24">
+      <c r="A3" s="23">
         <v>2</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="25" t="s">
         <v>33</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2138,10 +2167,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>35</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2149,10 +2178,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2160,32 +2189,32 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="24">
+      <c r="A7" s="23">
         <v>6</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>34</v>
+      <c r="B7" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="24">
+      <c r="A8" s="23">
         <v>7</v>
       </c>
-      <c r="B8" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>34</v>
+      <c r="B8" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2193,10 +2222,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2204,10 +2233,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2215,10 +2244,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2226,10 +2255,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2237,10 +2266,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2248,10 +2277,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2259,10 +2288,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2270,10 +2299,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2281,10 +2310,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2292,10 +2321,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2303,10 +2332,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2314,10 +2343,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2325,10 +2354,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2336,10 +2365,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2347,10 +2376,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2373,11 +2402,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2573,10 +2602,10 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2588,7 +2617,7 @@
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>21</v>
@@ -2606,7 +2635,7 @@
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>24</v>
@@ -2624,7 +2653,7 @@
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>21</v>
@@ -2642,7 +2671,7 @@
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" s="16" t="s">
         <v>22</v>
@@ -2660,18 +2689,18 @@
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="16" t="s">
         <v>31</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>32</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1">
@@ -2683,7 +2712,7 @@
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>27</v>
@@ -2691,10 +2720,10 @@
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="16" t="s">
         <v>35</v>
-      </c>
-      <c r="I16" s="16" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -2706,14 +2735,19 @@
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="5"/>
+      <c r="H17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
@@ -2724,7 +2758,7 @@
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E18" s="16" t="s">
         <v>27</v>
@@ -2732,10 +2766,10 @@
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="5" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -2743,36 +2777,31 @@
         <v>19</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>27</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
-      <c r="H19" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>36</v>
-      </c>
+      <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="5"/>
@@ -2782,14 +2811,14 @@
         <v>19</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -2800,14 +2829,14 @@
         <v>19</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -2818,14 +2847,14 @@
         <v>19</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
@@ -2836,14 +2865,14 @@
         <v>19</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -2854,31 +2883,33 @@
         <v>19</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="5"/>
+      <c r="E25" s="18" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="16" t="s">
-        <v>42</v>
-      </c>
       <c r="E26" s="18" t="s">
-        <v>24</v>
+        <v>31</v>
+      </c>
+      <c r="H26" t="s">
+        <v>41</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -2886,19 +2917,19 @@
         <v>19</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="E27" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H27" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="H27" t="s">
-        <v>43</v>
-      </c>
       <c r="I27" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -2906,19 +2937,13 @@
         <v>19</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="16" t="s">
-        <v>42</v>
-      </c>
       <c r="E28" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="H28" t="s">
-        <v>44</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -2926,13 +2951,19 @@
         <v>19</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="16" t="s">
-        <v>42</v>
-      </c>
       <c r="E29" s="18" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="H29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -2940,32 +2971,29 @@
         <v>19</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>36</v>
       </c>
       <c r="E30" s="18" t="s">
         <v>27</v>
       </c>
       <c r="H30" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E31" s="18" t="s">
+      <c r="B31" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2973,20 +3001,11 @@
       <c r="A32" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E32" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="H32" t="s">
-        <v>46</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>36</v>
+      <c r="B32" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -2994,7 +3013,7 @@
         <v>19</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C33" t="s">
         <v>21</v>
@@ -3005,10 +3024,10 @@
         <v>19</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C34" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -3016,9 +3035,12 @@
         <v>19</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" s="18" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3027,10 +3049,19 @@
         <v>19</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" t="s">
-        <v>24</v>
+        <v>43</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H36" t="s">
+        <v>45</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -3038,13 +3069,19 @@
         <v>19</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>21</v>
+        <v>27</v>
+      </c>
+      <c r="H37" t="s">
+        <v>75</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -3052,19 +3089,13 @@
         <v>19</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="H38" t="s">
-        <v>49</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -3072,19 +3103,13 @@
         <v>19</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="H39" t="s">
-        <v>50</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -3092,10 +3117,10 @@
         <v>19</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E40" s="18" t="s">
         <v>21</v>
@@ -3106,13 +3131,19 @@
         <v>19</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>22</v>
+        <v>27</v>
+      </c>
+      <c r="H41" t="s">
+        <v>76</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -3120,13 +3151,19 @@
         <v>19</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>36</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>21</v>
+        <v>27</v>
+      </c>
+      <c r="H42" t="s">
+        <v>77</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -3136,17 +3173,8 @@
       <c r="B43" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E43" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="H43" t="s">
-        <v>52</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>36</v>
+      <c r="C43" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -3156,11 +3184,8 @@
       <c r="B44" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D44" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E44" s="18" t="s">
-        <v>21</v>
+      <c r="C44" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -3170,17 +3195,8 @@
       <c r="B45" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D45" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E45" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="H45" t="s">
-        <v>53</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>36</v>
+      <c r="C45" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -3188,10 +3204,16 @@
         <v>19</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C46" t="s">
-        <v>21</v>
+        <v>31</v>
+      </c>
+      <c r="H46" t="s">
+        <v>48</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -3199,10 +3221,14 @@
         <v>19</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C47" t="s">
-        <v>23</v>
+        <v>47</v>
+      </c>
+      <c r="C47"/>
+      <c r="D47" t="s">
+        <v>50</v>
+      </c>
+      <c r="E47" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -3210,10 +3236,14 @@
         <v>19</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C48" t="s">
-        <v>21</v>
+        <v>47</v>
+      </c>
+      <c r="C48"/>
+      <c r="D48" t="s">
+        <v>50</v>
+      </c>
+      <c r="E48" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -3221,16 +3251,20 @@
         <v>19</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C49" t="s">
-        <v>32</v>
+        <v>47</v>
+      </c>
+      <c r="C49"/>
+      <c r="D49" t="s">
+        <v>50</v>
+      </c>
+      <c r="E49" t="s">
+        <v>27</v>
       </c>
       <c r="H49" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -3238,14 +3272,19 @@
         <v>19</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C50"/>
-      <c r="D50" t="s">
-        <v>57</v>
-      </c>
-      <c r="E50" t="s">
-        <v>21</v>
+        <v>47</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H50" t="s">
+        <v>78</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -3253,14 +3292,16 @@
         <v>19</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C51"/>
-      <c r="D51" t="s">
-        <v>57</v>
-      </c>
-      <c r="E51" t="s">
-        <v>22</v>
+        <v>52</v>
+      </c>
+      <c r="C51" t="s">
+        <v>27</v>
+      </c>
+      <c r="H51" t="s">
+        <v>53</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -3268,20 +3309,16 @@
         <v>19</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" t="s">
+        <v>27</v>
+      </c>
+      <c r="H52" t="s">
         <v>54</v>
       </c>
-      <c r="C52"/>
-      <c r="D52" t="s">
-        <v>57</v>
-      </c>
-      <c r="E52" t="s">
-        <v>27</v>
-      </c>
-      <c r="H52" t="s">
-        <v>58</v>
-      </c>
       <c r="I52" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -3289,13 +3326,16 @@
         <v>19</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D53" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E53" s="18" t="s">
-        <v>21</v>
+        <v>52</v>
+      </c>
+      <c r="C53" t="s">
+        <v>27</v>
+      </c>
+      <c r="H53" t="s">
+        <v>83</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -3303,136 +3343,54 @@
         <v>19</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D54" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E54" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C54" t="s">
         <v>27</v>
       </c>
       <c r="H54" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I54" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C55" s="19" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="A55" t="s">
-        <v>19</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C55" t="s">
-        <v>21</v>
+      <c r="D55" s="21"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="22" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" t="s">
-        <v>19</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C56" t="s">
-        <v>27</v>
-      </c>
-      <c r="H56" t="s">
-        <v>60</v>
-      </c>
-      <c r="I56" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
-      <c r="A57" t="s">
-        <v>19</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C57" t="s">
-        <v>27</v>
-      </c>
-      <c r="H57" t="s">
-        <v>61</v>
-      </c>
-      <c r="I57" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
-      <c r="A58" t="s">
-        <v>19</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C58" t="s">
-        <v>27</v>
-      </c>
-      <c r="H58" t="s">
-        <v>62</v>
-      </c>
-      <c r="I58" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
-      <c r="A59" t="s">
-        <v>19</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C59" t="s">
-        <v>27</v>
-      </c>
-      <c r="H59" t="s">
-        <v>63</v>
-      </c>
-      <c r="I59" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
-      <c r="A60" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B60" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C60" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="D60" s="22"/>
-      <c r="E60" s="22"/>
-      <c r="F60" s="22"/>
-      <c r="G60" s="22"/>
-      <c r="H60" s="19"/>
-      <c r="I60" s="23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
-      <c r="A61" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B61" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C61" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="D61" s="22"/>
-      <c r="E61" s="22"/>
-      <c r="F61" s="22"/>
-      <c r="G61" s="22"/>
-      <c r="H61" s="19"/>
-      <c r="I61" s="23" t="s">
-        <v>34</v>
+      <c r="A56" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="22" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CN_06_02 by Fausto Sáenz
Revisión de editor y ajustes de autor y corrector por cambios. Sin
cambios en mapa conceptual, cambia una imagen
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion02/EsqueletoGuion_CN_06_02_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion02/EsqueletoGuion_CN_06_02_CO.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="11760" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="11760" tabRatio="729" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725" iterateCount="2" iterateDelta="10"/>
+  <calcPr calcId="144525" iterateCount="2" iterateDelta="10"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="90">
   <si>
     <t>FICHA</t>
   </si>
@@ -118,9 +118,6 @@
     <t>Estructura celular</t>
   </si>
   <si>
-    <t>Los organelos celulares y sus funciones</t>
-  </si>
-  <si>
     <t>Profundiza</t>
   </si>
   <si>
@@ -287,13 +284,25 @@
   </si>
   <si>
     <t>Fin de tema</t>
+  </si>
+  <si>
+    <t>Los orgánulos celulares y sus funciones</t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t>Observación en el microscopio de células animales y vegetales</t>
+  </si>
+  <si>
+    <t>Competencias: Observación en el microscopio de células animales y vegetales</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -810,7 +819,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -821,9 +830,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1544,65 +1550,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="2" width="132" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="15" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1617,14 +1623,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.28515625" customWidth="1"/>
@@ -1636,41 +1642,41 @@
     <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" t="s">
         <v>67</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" t="s">
-        <v>68</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1682,329 +1688,407 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
         <v>63</v>
       </c>
-      <c r="B3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
         <v>64</v>
-      </c>
-      <c r="D3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" t="s">
-        <v>65</v>
       </c>
       <c r="F3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
         <v>69</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>70</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
         <v>71</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" t="s">
-        <v>72</v>
       </c>
       <c r="F4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" t="s">
         <v>67</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" t="s">
-        <v>68</v>
       </c>
       <c r="F5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
         <v>63</v>
       </c>
-      <c r="B6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
         <v>64</v>
-      </c>
-      <c r="D6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" t="s">
-        <v>65</v>
       </c>
       <c r="F6">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" t="s">
         <v>67</v>
-      </c>
-      <c r="C7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" t="s">
-        <v>68</v>
       </c>
       <c r="F7">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
         <v>67</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" t="s">
-        <v>68</v>
       </c>
       <c r="F8">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" t="s">
         <v>67</v>
-      </c>
-      <c r="C9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" t="s">
-        <v>68</v>
       </c>
       <c r="F9">
         <v>11</v>
       </c>
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="G9" s="9"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" t="s">
         <v>67</v>
-      </c>
-      <c r="C10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" t="s">
-        <v>68</v>
       </c>
       <c r="F10">
         <v>12</v>
       </c>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
       <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" t="s">
         <v>67</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" t="s">
-        <v>68</v>
       </c>
       <c r="F11">
         <v>13</v>
       </c>
-      <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
       <c r="B12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" t="s">
         <v>67</v>
-      </c>
-      <c r="C12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" t="s">
-        <v>68</v>
       </c>
       <c r="F12">
         <v>14</v>
       </c>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
       <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" t="s">
         <v>67</v>
-      </c>
-      <c r="C13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" t="s">
-        <v>68</v>
       </c>
       <c r="F13">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
       <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" t="s">
         <v>67</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" t="s">
-        <v>68</v>
       </c>
       <c r="F14">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
       <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" t="s">
         <v>67</v>
-      </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" t="s">
-        <v>68</v>
       </c>
       <c r="F15">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6</v>
       </c>
       <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" t="s">
         <v>67</v>
-      </c>
-      <c r="C16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" t="s">
-        <v>68</v>
       </c>
       <c r="F16">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6</v>
       </c>
       <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" t="s">
         <v>67</v>
       </c>
-      <c r="C17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" t="s">
-        <v>68</v>
-      </c>
       <c r="F17">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
       <c r="B18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" t="s">
         <v>67</v>
-      </c>
-      <c r="C18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" t="s">
-        <v>84</v>
-      </c>
-      <c r="E18" t="s">
-        <v>68</v>
       </c>
       <c r="F18">
         <v>20</v>
       </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D26" s="16"/>
+      <c r="E26" s="15"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D27" s="5"/>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D28" s="5"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="5"/>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="5"/>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="5"/>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E42" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2018,83 +2102,83 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="66.140625" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1">
-      <c r="A5" s="19" t="s">
-        <v>58</v>
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="19" t="s">
-        <v>57</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2112,278 +2196,319 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="92.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="23">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="22">
         <v>2</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="23">
+        <v>72</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="22">
         <v>6</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="22">
+        <v>7</v>
+      </c>
+      <c r="B8" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="23">
-        <v>7</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="C8" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>82</v>
-      </c>
       <c r="C20" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="19">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="19">
+      <c r="B22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="18">
         <v>22</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="C27" s="6"/>
+      <c r="C23" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="18">
+        <v>23</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="5"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="5"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="5"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="5"/>
     </row>
   </sheetData>
   <sortState ref="A2:C38">
@@ -2401,15 +2526,15 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.7109375" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" style="2" customWidth="1"/>
@@ -2422,36 +2547,36 @@
     <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2461,13 +2586,13 @@
       <c r="C2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2477,13 +2602,13 @@
       <c r="C3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2493,13 +2618,13 @@
       <c r="C4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2509,13 +2634,13 @@
       <c r="C5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2525,872 +2650,918 @@
       <c r="C6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="16" t="s">
+      <c r="C7" s="7"/>
+      <c r="D7" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="16" t="s">
+      <c r="C8" s="7"/>
+      <c r="D8" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="16" t="s">
+      <c r="C9" s="7"/>
+      <c r="D9" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="16" t="s">
+      <c r="C10" s="7"/>
+      <c r="D10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
       <c r="H10" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="16" t="s">
+      <c r="C11" s="7"/>
+      <c r="D11" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="16" t="s">
+      <c r="C12" s="7"/>
+      <c r="D12" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1">
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="16" t="s">
+      <c r="C13" s="7"/>
+      <c r="D13" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1">
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="16" t="s">
+      <c r="C14" s="7"/>
+      <c r="D14" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="13.5" customHeight="1">
+    <row r="15" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="16" t="s">
+      <c r="C15" s="7"/>
+      <c r="D15" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="5" t="s">
+      <c r="I15" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="I15" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1">
+    </row>
+    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="16" t="s">
+      <c r="C16" s="7"/>
+      <c r="D16" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="17" t="s">
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="16" t="s">
+      <c r="C17" s="7"/>
+      <c r="D17" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="I17" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="16" t="s">
+      <c r="C18" s="7"/>
+      <c r="D18" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
       <c r="H18" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>72</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="16" t="s">
+      <c r="E20" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E22" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="16" t="s">
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E23" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="16" t="s">
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="I26" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" t="s">
         <v>41</v>
       </c>
-      <c r="I26" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="I27" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H29" t="s">
+        <v>36</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H30" t="s">
+        <v>73</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="H29" t="s">
-        <v>37</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D30" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="H30" t="s">
-        <v>74</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="C31" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>19</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C33" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>19</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C34" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>19</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="E35" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="18" t="s">
+      <c r="I36" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H38" t="s">
+        <v>74</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E39" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
-      <c r="A36" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E36" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H36" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I36" s="5" t="s">
+      <c r="E40" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H42" t="s">
+        <v>75</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="17" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" t="s">
-        <v>19</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E37" s="18" t="s">
+      <c r="E43" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="H37" t="s">
-        <v>75</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D38" s="3" t="s">
+      <c r="H43" t="s">
+        <v>76</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E38" s="18" t="s">
+      <c r="C44" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
-      <c r="A39" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D39" s="3" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E39" s="18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" t="s">
-        <v>19</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D40" s="3" t="s">
+      <c r="C45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E40" s="18" t="s">
+      <c r="C46" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
-      <c r="A41" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D41" s="3" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E41" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="H41" t="s">
-        <v>76</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D42" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E42" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="H42" t="s">
-        <v>77</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" t="s">
-        <v>19</v>
-      </c>
-      <c r="B43" s="2" t="s">
+      <c r="C47" t="s">
+        <v>30</v>
+      </c>
+      <c r="H47" t="s">
         <v>47</v>
       </c>
-      <c r="C43" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" t="s">
-        <v>19</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C44" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" t="s">
-        <v>19</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C45" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" t="s">
-        <v>19</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C46" t="s">
-        <v>31</v>
-      </c>
-      <c r="H46" t="s">
+      <c r="I47" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I46" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" t="s">
-        <v>19</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C47"/>
-      <c r="D47" t="s">
-        <v>50</v>
-      </c>
-      <c r="E47" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>19</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C48"/>
       <c r="D48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E48" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>19</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C49"/>
       <c r="D49" t="s">
+        <v>49</v>
+      </c>
+      <c r="E49" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C50"/>
+      <c r="D50" t="s">
+        <v>49</v>
+      </c>
+      <c r="E50" t="s">
+        <v>27</v>
+      </c>
+      <c r="H50" t="s">
         <v>50</v>
       </c>
-      <c r="E49" t="s">
+      <c r="I50" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C51"/>
+      <c r="D51" t="s">
+        <v>49</v>
+      </c>
+      <c r="E51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D52" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E52" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H52" t="s">
+        <v>77</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" t="s">
-        <v>19</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D50" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E50" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="H50" t="s">
-        <v>78</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" t="s">
-        <v>19</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C51" t="s">
-        <v>27</v>
-      </c>
-      <c r="H51" t="s">
-        <v>53</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
-      <c r="A52" t="s">
-        <v>19</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C52" t="s">
-        <v>27</v>
-      </c>
-      <c r="H52" t="s">
-        <v>54</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
-      <c r="A53" t="s">
-        <v>19</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="C53" t="s">
         <v>27</v>
       </c>
       <c r="H53" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>19</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C54" t="s">
         <v>27</v>
       </c>
       <c r="H54" t="s">
+        <v>53</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C55" t="s">
+        <v>27</v>
+      </c>
+      <c r="H55" t="s">
+        <v>82</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C56" t="s">
+        <v>27</v>
+      </c>
+      <c r="H56" t="s">
+        <v>88</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C57" t="s">
+        <v>27</v>
+      </c>
+      <c r="H57" t="s">
+        <v>54</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C58" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="I54" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="A55" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B55" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C55" s="19" t="s">
+      <c r="D58" s="20"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="18"/>
+      <c r="I58" s="21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C59" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D55" s="21"/>
-      <c r="E55" s="21"/>
-      <c r="F55" s="21"/>
-      <c r="G55" s="21"/>
-      <c r="H55" s="19"/>
-      <c r="I55" s="22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="A56" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B56" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C56" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="D56" s="21"/>
-      <c r="E56" s="21"/>
-      <c r="F56" s="21"/>
-      <c r="G56" s="21"/>
-      <c r="H56" s="19"/>
-      <c r="I56" s="22" t="s">
-        <v>33</v>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="18"/>
+      <c r="I59" s="21" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrección de errores en esqueleto del guión
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion02/EsqueletoGuion_CN_06_02_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion02/EsqueletoGuion_CN_06_02_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="11760" tabRatio="729" activeTab="3"/>
+    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="11760" tabRatio="729" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525" iterateCount="2" iterateDelta="10"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="85">
   <si>
     <t>FICHA</t>
   </si>
@@ -184,15 +184,6 @@
     <t>Competencias</t>
   </si>
   <si>
-    <t>Construcción de los distintos modelos celulares</t>
-  </si>
-  <si>
-    <t>Preparación de una muestra para el microscopio</t>
-  </si>
-  <si>
-    <t>Utilización del microscopio y la lupa binocular</t>
-  </si>
-  <si>
     <t>Mapa conceptual</t>
   </si>
   <si>
@@ -274,9 +265,6 @@
     <t>Competencias: diferenciación del tipo celular al microscopio</t>
   </si>
   <si>
-    <t>Diferenciación del tipo celular al microscopio</t>
-  </si>
-  <si>
     <t>Competencias: utilización del microscopio y la lupa binocular</t>
   </si>
   <si>
@@ -292,10 +280,7 @@
     <t>si</t>
   </si>
   <si>
-    <t>Observación en el microscopio de células animales y vegetales</t>
-  </si>
-  <si>
-    <t>Competencias: Observación en el microscopio de células animales y vegetales</t>
+    <t>Competencias: comparación entre células vegetales y animales</t>
   </si>
 </sst>
 </file>
@@ -1543,7 +1528,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1576,7 +1561,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1584,7 +1569,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1592,7 +1577,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1608,7 +1593,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1626,8 +1611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1667,16 +1652,16 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1690,19 +1675,19 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
         <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -1710,19 +1695,19 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
         <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F4">
         <v>4</v>
@@ -1733,16 +1718,16 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
         <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F5">
         <v>5</v>
@@ -1750,19 +1735,19 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D6" t="s">
         <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F6">
         <v>8</v>
@@ -1773,16 +1758,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C7" t="s">
         <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F7">
         <v>9</v>
@@ -1793,7 +1778,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
         <v>40</v>
@@ -1802,7 +1787,7 @@
         <v>44</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F8">
         <v>10</v>
@@ -1813,16 +1798,16 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
         <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F9">
         <v>11</v>
@@ -1834,16 +1819,16 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
         <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F10">
         <v>12</v>
@@ -1855,16 +1840,16 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
         <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F11">
         <v>13</v>
@@ -1876,7 +1861,7 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
         <v>40</v>
@@ -1885,7 +1870,7 @@
         <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F12">
         <v>14</v>
@@ -1897,7 +1882,7 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
         <v>40</v>
@@ -1906,7 +1891,7 @@
         <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F13">
         <v>15</v>
@@ -1917,16 +1902,16 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
         <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E14" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F14">
         <v>16</v>
@@ -1937,16 +1922,16 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
         <v>40</v>
       </c>
       <c r="D15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F15">
         <v>17</v>
@@ -1957,16 +1942,16 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
         <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F16">
         <v>18</v>
@@ -1977,16 +1962,16 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
         <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F17">
         <v>19</v>
@@ -1997,16 +1982,16 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
         <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F18">
         <v>20</v>
@@ -2017,16 +2002,16 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
         <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E19" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F19">
         <v>21</v>
@@ -2161,7 +2146,7 @@
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
@@ -2172,7 +2157,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
         <v>32</v>
@@ -2202,8 +2187,8 @@
   </sheetPr>
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2229,7 +2214,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>28</v>
@@ -2273,7 +2258,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>34</v>
@@ -2317,7 +2302,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>34</v>
@@ -2339,7 +2324,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>34</v>
@@ -2350,7 +2335,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>34</v>
@@ -2361,7 +2346,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>34</v>
@@ -2394,7 +2379,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>48</v>
@@ -2405,7 +2390,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>48</v>
@@ -2416,7 +2401,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>48</v>
@@ -2427,7 +2412,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>48</v>
@@ -2438,7 +2423,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>48</v>
@@ -2449,7 +2434,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>48</v>
@@ -2460,7 +2445,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C23" s="19" t="s">
         <v>32</v>
@@ -2471,7 +2456,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C24" s="19" t="s">
         <v>32</v>
@@ -2530,8 +2515,8 @@
   <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2727,7 +2712,7 @@
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>28</v>
@@ -2778,7 +2763,7 @@
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>21</v>
@@ -2796,7 +2781,7 @@
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>22</v>
@@ -2814,7 +2799,7 @@
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>30</v>
@@ -2837,7 +2822,7 @@
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>27</v>
@@ -2891,7 +2876,7 @@
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>34</v>
@@ -3105,7 +3090,7 @@
         <v>27</v>
       </c>
       <c r="H30" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I30" s="5" t="s">
         <v>34</v>
@@ -3217,7 +3202,7 @@
         <v>27</v>
       </c>
       <c r="H38" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I38" s="5" t="s">
         <v>34</v>
@@ -3279,7 +3264,7 @@
         <v>27</v>
       </c>
       <c r="H42" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I42" s="5" t="s">
         <v>34</v>
@@ -3299,7 +3284,7 @@
         <v>27</v>
       </c>
       <c r="H43" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>34</v>
@@ -3435,7 +3420,7 @@
         <v>27</v>
       </c>
       <c r="H52" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I52" s="5" t="s">
         <v>48</v>
@@ -3452,7 +3437,7 @@
         <v>27</v>
       </c>
       <c r="H53" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="I53" s="5" t="s">
         <v>48</v>
@@ -3469,7 +3454,7 @@
         <v>27</v>
       </c>
       <c r="H54" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="I54" s="5" t="s">
         <v>48</v>
@@ -3486,7 +3471,7 @@
         <v>27</v>
       </c>
       <c r="H55" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>48</v>
@@ -3503,10 +3488,10 @@
         <v>27</v>
       </c>
       <c r="H56" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3520,7 +3505,7 @@
         <v>27</v>
       </c>
       <c r="H57" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>48</v>
@@ -3531,10 +3516,10 @@
         <v>19</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D58" s="20"/>
       <c r="E58" s="20"/>
@@ -3550,10 +3535,10 @@
         <v>19</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D59" s="20"/>
       <c r="E59" s="20"/>

</xml_diff>

<commit_message>
CN0602: Ajuste de Esqueleto de guion y carga de archivo de seguimiento de producción digital
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion02/EsqueletoGuion_CN_06_02_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion02/EsqueletoGuion_CN_06_02_CO.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\CienciasNaturales\fuentes\contenidos\grado06\guion02\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="11760" tabRatio="729" activeTab="1"/>
+    <workbookView xWindow="3408" yWindow="1395" windowWidth="19444" windowHeight="11761" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -15,18 +20,18 @@
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="84">
   <si>
     <t>FICHA</t>
   </si>
@@ -257,9 +262,6 @@
   </si>
   <si>
     <t>Competencias: preparación de una muestra para el microscopio</t>
-  </si>
-  <si>
-    <t>Competencias: Preparación de una muestra para el microscopio</t>
   </si>
   <si>
     <t>Competencias: diferenciación del tipo celular al microscopio</t>
@@ -1528,7 +1530,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1538,17 +1540,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
     <col min="2" max="2" width="132" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="14" t="s">
         <v>8</v>
       </c>
@@ -1556,7 +1558,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
         <v>9</v>
       </c>
@@ -1564,15 +1566,15 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
         <v>11</v>
       </c>
@@ -1580,7 +1582,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
         <v>1</v>
       </c>
@@ -1588,7 +1590,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
         <v>12</v>
       </c>
@@ -1611,23 +1613,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" customWidth="1"/>
-    <col min="4" max="4" width="77.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.265625" customWidth="1"/>
+    <col min="4" max="4" width="77.265625" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
@@ -1647,7 +1649,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>6</v>
       </c>
@@ -1673,7 +1675,7 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -1693,7 +1695,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -1713,7 +1715,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>6</v>
       </c>
@@ -1733,7 +1735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -1753,7 +1755,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1773,7 +1775,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1793,7 +1795,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1814,7 +1816,7 @@
       </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1835,7 +1837,7 @@
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>6</v>
       </c>
@@ -1856,7 +1858,7 @@
       </c>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1877,7 +1879,7 @@
       </c>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1897,7 +1899,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1917,7 +1919,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>6</v>
       </c>
@@ -1937,7 +1939,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>6</v>
       </c>
@@ -1957,7 +1959,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>6</v>
       </c>
@@ -1968,7 +1970,7 @@
         <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E17" t="s">
         <v>64</v>
@@ -1977,7 +1979,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>6</v>
       </c>
@@ -1988,7 +1990,7 @@
         <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E18" t="s">
         <v>64</v>
@@ -1997,7 +1999,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>6</v>
       </c>
@@ -2008,7 +2010,7 @@
         <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E19" t="s">
         <v>64</v>
@@ -2017,62 +2019,62 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D26" s="16"/>
       <c r="E26" s="15"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D27" s="5"/>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D28" s="5"/>
       <c r="E28" s="8"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E37" s="5"/>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E38" s="5"/>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E39" s="5"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E40" s="5"/>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E41" s="5"/>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E42" s="5"/>
     </row>
   </sheetData>
@@ -2094,13 +2096,13 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="66.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="66.1328125" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
@@ -2111,7 +2113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>31</v>
       </c>
@@ -2122,7 +2124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -2133,7 +2135,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -2144,7 +2146,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="18" t="s">
         <v>54</v>
       </c>
@@ -2155,7 +2157,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="18" t="s">
         <v>53</v>
       </c>
@@ -2182,23 +2184,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="92.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.265625" customWidth="1"/>
+    <col min="3" max="3" width="19.265625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
@@ -2209,7 +2211,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2220,7 +2222,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="22">
         <v>2</v>
       </c>
@@ -2231,7 +2233,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2242,7 +2244,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2253,7 +2255,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2264,7 +2266,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="22">
         <v>6</v>
       </c>
@@ -2275,7 +2277,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="22">
         <v>7</v>
       </c>
@@ -2286,7 +2288,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2297,7 +2299,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2308,7 +2310,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2319,7 +2321,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2330,7 +2332,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2341,7 +2343,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2352,7 +2354,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2363,7 +2365,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2374,7 +2376,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2385,7 +2387,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2396,51 +2398,51 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="18">
         <v>22</v>
       </c>
@@ -2451,7 +2453,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="18">
         <v>23</v>
       </c>
@@ -2462,37 +2464,37 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C35" s="5"/>
     </row>
   </sheetData>
@@ -2515,24 +2517,24 @@
   <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H57" sqref="H57"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="35.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="68.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.73046875" customWidth="1"/>
+    <col min="2" max="2" width="36.73046875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.1328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="35.59765625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.3984375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17.86328125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.1328125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="68.59765625" customWidth="1"/>
+    <col min="9" max="9" width="17.3984375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
@@ -2561,7 +2563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2577,7 +2579,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2593,7 +2595,7 @@
       <c r="G3" s="8"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2609,7 +2611,7 @@
       <c r="G4" s="8"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2625,7 +2627,7 @@
       <c r="G5" s="8"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2641,7 +2643,7 @@
       <c r="G6" s="8"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2659,7 +2661,7 @@
       <c r="G7" s="8"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -2677,7 +2679,7 @@
       <c r="G8" s="8"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -2695,7 +2697,7 @@
       <c r="G9" s="8"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2718,7 +2720,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2736,7 +2738,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2754,7 +2756,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2763,7 +2765,7 @@
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>21</v>
@@ -2772,7 +2774,7 @@
       <c r="G13" s="8"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2781,7 +2783,7 @@
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>22</v>
@@ -2790,7 +2792,7 @@
       <c r="G14" s="8"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -2799,7 +2801,7 @@
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>30</v>
@@ -2813,7 +2815,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -2822,7 +2824,7 @@
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>27</v>
@@ -2836,7 +2838,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2859,7 +2861,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -2882,7 +2884,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2898,7 +2900,7 @@
       <c r="G19" s="8"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2916,7 +2918,7 @@
       <c r="G20" s="8"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2934,7 +2936,7 @@
       <c r="G21" s="8"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -2952,7 +2954,7 @@
       <c r="G22" s="8"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2970,7 +2972,7 @@
       <c r="G23" s="8"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2988,7 +2990,7 @@
       <c r="G24" s="8"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -3002,7 +3004,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -3022,7 +3024,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -3042,7 +3044,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -3056,7 +3058,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -3076,7 +3078,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -3096,7 +3098,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -3107,7 +3109,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -3118,7 +3120,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -3129,7 +3131,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -3140,7 +3142,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -3154,7 +3156,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -3174,7 +3176,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>19</v>
       </c>
@@ -3188,7 +3190,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -3208,7 +3210,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -3222,7 +3224,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -3236,7 +3238,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -3250,7 +3252,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -3270,7 +3272,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -3290,7 +3292,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -3301,7 +3303,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>19</v>
       </c>
@@ -3312,7 +3314,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>19</v>
       </c>
@@ -3323,7 +3325,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>19</v>
       </c>
@@ -3340,7 +3342,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>19</v>
       </c>
@@ -3355,7 +3357,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>19</v>
       </c>
@@ -3370,7 +3372,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>19</v>
       </c>
@@ -3391,7 +3393,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>19</v>
       </c>
@@ -3406,7 +3408,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>19</v>
       </c>
@@ -3426,7 +3428,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>19</v>
       </c>
@@ -3443,7 +3445,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -3460,7 +3462,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>19</v>
       </c>
@@ -3471,13 +3473,13 @@
         <v>27</v>
       </c>
       <c r="H55" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>19</v>
       </c>
@@ -3488,13 +3490,13 @@
         <v>27</v>
       </c>
       <c r="H56" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>19</v>
       </c>
@@ -3505,18 +3507,18 @@
         <v>27</v>
       </c>
       <c r="H57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C58" s="18" t="s">
         <v>52</v>
@@ -3530,12 +3532,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C59" s="18" t="s">
         <v>53</v>

</xml_diff>